<commit_message>
Tariff Added in table
</commit_message>
<xml_diff>
--- a/public/downloads/sample.xlsx
+++ b/public/downloads/sample.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\orca-billing\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FC67921-A3C7-4105-B8A6-26E5390C3060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CBBC2C-2C39-498D-AAA9-BD68BF8187B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
+  <calcPr calcId="181029" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>2019-11-25 15:36:13</t>
   </si>
@@ -60,15 +60,9 @@
     <t>From Day</t>
   </si>
   <si>
-    <t>To Day</t>
-  </si>
-  <si>
     <t>From Hour</t>
   </si>
   <si>
-    <t>To Hour</t>
-  </si>
-  <si>
     <t>Grace Period</t>
   </si>
   <si>
@@ -91,19 +85,60 @@
   </si>
   <si>
     <t xml:space="preserve">Do </t>
+  </si>
+  <si>
+    <t>To Day (Must be greater than From Day)</t>
+  </si>
+  <si>
+    <t>To Hour  (Must be greater than From Hour)</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -130,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -139,6 +174,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -445,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +501,10 @@
     <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -471,50 +515,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -531,15 +575,15 @@
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
         <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>700</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="5">
         <v>2100</v>
       </c>
       <c r="I2" s="1">
@@ -577,13 +621,13 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>3</v>
       </c>
       <c r="G3" s="1">
         <v>700</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <v>2100</v>
       </c>
       <c r="I3" s="1">
@@ -621,13 +665,13 @@
       <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
+      <c r="F4" s="5">
+        <v>6</v>
       </c>
       <c r="G4" s="1">
         <v>700</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="5">
         <v>2100</v>
       </c>
       <c r="I4" s="1">
@@ -650,22 +694,78 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>